<commit_message>
Export knot number tables and updated doc
</commit_message>
<xml_diff>
--- a/doc/Document Tables.xlsx
+++ b/doc/Document Tables.xlsx
@@ -1,13 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\nmfs.local\AKC-ABL\Users\curry.cunningham\My Documents\Projects\VAST Evaluation\AFSC_VAST_Evaluation\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="38480" yWindow="-1480" windowWidth="24480" windowHeight="17260" tabRatio="500"/>
+    <workbookView xWindow="38475" yWindow="-1485" windowWidth="24480" windowHeight="17265" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Species" sheetId="1" r:id="rId1"/>
+    <sheet name="CVs" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Species!$A$1:$C$1</definedName>
@@ -22,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="27">
   <si>
     <t>Region</t>
   </si>
@@ -97,13 +103,19 @@
   </si>
   <si>
     <t>Pleurogrammus monopterygius</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>VAST Model Knot Specification (n_x)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -143,6 +155,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -161,7 +180,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="12">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -174,13 +193,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="12" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="12">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -193,8 +225,26 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="12" builtinId="5"/>
   </cellStyles>
   <dxfs count="2">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -212,33 +262,24 @@
         <scheme val="minor"/>
       </font>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C15" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C15" totalsRowShown="0" headerRowDxfId="1">
   <tableColumns count="3">
     <tableColumn id="1" name="Common Name"/>
-    <tableColumn id="2" name="Scientific Name" dataDxfId="1"/>
+    <tableColumn id="2" name="Scientific Name" dataDxfId="0"/>
     <tableColumn id="3" name="Region"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -569,18 +610,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.1640625" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.125" customWidth="1"/>
+    <col min="2" max="2" width="29.625" customWidth="1"/>
+    <col min="3" max="3" width="14.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -591,7 +632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -602,7 +643,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -613,7 +654,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -624,7 +665,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -635,7 +676,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -646,7 +687,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -657,7 +698,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -668,7 +709,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -679,7 +720,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -690,7 +731,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -701,7 +742,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -712,7 +753,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -723,7 +764,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -734,7 +775,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -757,4 +798,489 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:H22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:H22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="5">
+        <v>100</v>
+      </c>
+      <c r="C4" s="5">
+        <v>200</v>
+      </c>
+      <c r="D4" s="5">
+        <v>300</v>
+      </c>
+      <c r="E4" s="5">
+        <v>400</v>
+      </c>
+      <c r="F4" s="5">
+        <v>500</v>
+      </c>
+      <c r="G4" s="5">
+        <v>750</v>
+      </c>
+      <c r="H4" s="5">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="6">
+        <v>-0.172033666650799</v>
+      </c>
+      <c r="C5" s="6">
+        <v>-0.21167461660944001</v>
+      </c>
+      <c r="D5" s="6">
+        <v>-0.20215163545793099</v>
+      </c>
+      <c r="E5" s="6">
+        <v>-0.20646862752263401</v>
+      </c>
+      <c r="F5" s="6">
+        <v>-0.21744322095305699</v>
+      </c>
+      <c r="G5" s="6">
+        <v>-0.225574064860074</v>
+      </c>
+      <c r="H5" s="6">
+        <v>-0.23320697566235099</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="6">
+        <v>-0.11659698793617999</v>
+      </c>
+      <c r="C6" s="6">
+        <v>-4.6655320264011903E-2</v>
+      </c>
+      <c r="D6" s="6">
+        <v>-8.2071749580468895E-2</v>
+      </c>
+      <c r="E6" s="6">
+        <v>-7.0225716441070701E-2</v>
+      </c>
+      <c r="F6" s="6">
+        <v>-4.9467660840880397E-2</v>
+      </c>
+      <c r="G6" s="6">
+        <v>-5.8881687623085703E-2</v>
+      </c>
+      <c r="H6" s="6">
+        <v>-7.9344830269770197E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="6">
+        <v>-0.47735462967118802</v>
+      </c>
+      <c r="C7" s="6">
+        <v>-0.47823423372074902</v>
+      </c>
+      <c r="D7" s="6">
+        <v>-0.48075111949067401</v>
+      </c>
+      <c r="E7" s="6">
+        <v>-0.47969377920014999</v>
+      </c>
+      <c r="F7" s="6">
+        <v>-0.48327084038687801</v>
+      </c>
+      <c r="G7" s="6">
+        <v>-0.48347441893728699</v>
+      </c>
+      <c r="H7" s="6">
+        <v>-0.484178785114243</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="6">
+        <v>-0.42336225116582099</v>
+      </c>
+      <c r="C8" s="6">
+        <v>-0.42978829226184401</v>
+      </c>
+      <c r="D8" s="6">
+        <v>-0.43054175017481</v>
+      </c>
+      <c r="E8" s="6">
+        <v>-0.43857799323670599</v>
+      </c>
+      <c r="F8" s="6">
+        <v>-0.4325395597992</v>
+      </c>
+      <c r="G8" s="6">
+        <v>-0.41979056694823302</v>
+      </c>
+      <c r="H8" s="6">
+        <v>-0.43260419909207998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="6">
+        <v>-4.63700074382081E-2</v>
+      </c>
+      <c r="C9" s="6">
+        <v>-6.8470506145828003E-2</v>
+      </c>
+      <c r="D9" s="6">
+        <v>-8.7998193871509006E-2</v>
+      </c>
+      <c r="E9" s="6">
+        <v>-0.106271905976751</v>
+      </c>
+      <c r="F9" s="6">
+        <v>-9.2243110105519804E-2</v>
+      </c>
+      <c r="G9" s="6">
+        <v>-0.11261745542922399</v>
+      </c>
+      <c r="H9" s="6">
+        <v>-0.11081741659528301</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="6">
+        <v>-7.5076824332551306E-2</v>
+      </c>
+      <c r="C10" s="6">
+        <v>-8.1504796751249803E-2</v>
+      </c>
+      <c r="D10" s="6">
+        <v>-9.2203344242930099E-2</v>
+      </c>
+      <c r="E10" s="6">
+        <v>-9.3549026531111995E-2</v>
+      </c>
+      <c r="F10" s="6">
+        <v>-9.1131987033842399E-2</v>
+      </c>
+      <c r="G10" s="6">
+        <v>-9.63153176291906E-2</v>
+      </c>
+      <c r="H10" s="6">
+        <v>-0.100478582932572</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="6">
+        <v>-0.30128172079058801</v>
+      </c>
+      <c r="C11" s="6">
+        <v>-0.30349258612034902</v>
+      </c>
+      <c r="D11" s="6">
+        <v>-0.30685264037614002</v>
+      </c>
+      <c r="E11" s="6">
+        <v>-0.31988988759741599</v>
+      </c>
+      <c r="F11" s="6">
+        <v>-0.31431787058965199</v>
+      </c>
+      <c r="G11" s="6">
+        <v>-0.32794109500630803</v>
+      </c>
+      <c r="H11" s="6">
+        <v>-0.31664385632049902</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="6">
+        <v>-8.1356792970777206E-2</v>
+      </c>
+      <c r="C12" s="6">
+        <v>-9.7225086063537497E-2</v>
+      </c>
+      <c r="D12" s="6">
+        <v>-0.10581610184028099</v>
+      </c>
+      <c r="E12" s="6">
+        <v>-0.110560470416739</v>
+      </c>
+      <c r="F12" s="6">
+        <v>-0.12714521863946401</v>
+      </c>
+      <c r="G12" s="6">
+        <v>-0.13859479025957</v>
+      </c>
+      <c r="H12" s="6">
+        <v>-0.14532068629028799</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="6">
+        <v>-0.45614395311852701</v>
+      </c>
+      <c r="C13" s="6">
+        <v>-0.46445351724316702</v>
+      </c>
+      <c r="D13" s="6">
+        <v>-0.46712276524546797</v>
+      </c>
+      <c r="E13" s="6">
+        <v>-0.47122980070753501</v>
+      </c>
+      <c r="F13" s="6">
+        <v>-0.474878173128717</v>
+      </c>
+      <c r="G13" s="6">
+        <v>-0.47602537920932803</v>
+      </c>
+      <c r="H13" s="6">
+        <v>-0.47504208961909999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="5">
+        <v>100</v>
+      </c>
+      <c r="C17" s="5">
+        <v>200</v>
+      </c>
+      <c r="D17" s="5">
+        <v>300</v>
+      </c>
+      <c r="E17" s="5">
+        <v>400</v>
+      </c>
+      <c r="F17" s="5">
+        <v>500</v>
+      </c>
+      <c r="G17" s="5">
+        <v>750</v>
+      </c>
+      <c r="H17" s="5">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="6">
+        <v>0.40206667874438501</v>
+      </c>
+      <c r="C18" s="6">
+        <v>0.35372882267482703</v>
+      </c>
+      <c r="D18" s="6">
+        <v>0.279645426709414</v>
+      </c>
+      <c r="E18" s="6">
+        <v>0.24555450887570501</v>
+      </c>
+      <c r="F18" s="6">
+        <v>0.181530435316685</v>
+      </c>
+      <c r="G18" s="6">
+        <v>0.21593836237153999</v>
+      </c>
+      <c r="H18" s="6">
+        <v>0.21721569551438</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="6">
+        <v>-8.8910240495234001E-3</v>
+      </c>
+      <c r="C19" s="6">
+        <v>6.6898104923970997E-2</v>
+      </c>
+      <c r="D19" s="6">
+        <v>-8.7022934231200805E-2</v>
+      </c>
+      <c r="E19" s="6">
+        <v>-3.8570188579889399E-2</v>
+      </c>
+      <c r="F19" s="6">
+        <v>-5.82454321445025E-2</v>
+      </c>
+      <c r="G19" s="6">
+        <v>-8.5155917447454793E-2</v>
+      </c>
+      <c r="H19" s="6">
+        <v>-0.10999567398181399</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="6">
+        <v>-0.249847546068524</v>
+      </c>
+      <c r="C20" s="6">
+        <v>-0.22393092816979901</v>
+      </c>
+      <c r="D20" s="6">
+        <v>-0.20901627755773999</v>
+      </c>
+      <c r="E20" s="6">
+        <v>-0.23995942732798201</v>
+      </c>
+      <c r="F20" s="6">
+        <v>-0.216851520715201</v>
+      </c>
+      <c r="G20" s="6">
+        <v>-0.18802173950006901</v>
+      </c>
+      <c r="H20" s="6">
+        <v>-0.13592893757511301</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="6">
+        <v>-7.6866319208249698E-2</v>
+      </c>
+      <c r="C21" s="6">
+        <v>-0.10581985445785</v>
+      </c>
+      <c r="D21" s="6">
+        <v>-9.0342215364723005E-2</v>
+      </c>
+      <c r="E21" s="6">
+        <v>-7.5435209305558804E-2</v>
+      </c>
+      <c r="F21" s="6">
+        <v>-3.9874213705633502E-2</v>
+      </c>
+      <c r="G21" s="6">
+        <v>-7.4631440661902596E-2</v>
+      </c>
+      <c r="H21" s="6">
+        <v>-1.3432919863705199E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="6">
+        <v>0.288065075752998</v>
+      </c>
+      <c r="C22" s="6">
+        <v>0.49599574455914802</v>
+      </c>
+      <c r="D22" s="6">
+        <v>0.47802532940015202</v>
+      </c>
+      <c r="E22" s="6">
+        <v>0.49216163355298398</v>
+      </c>
+      <c r="F22" s="6">
+        <v>0.49459423842366501</v>
+      </c>
+      <c r="G22" s="6">
+        <v>0.52037926494853104</v>
+      </c>
+      <c r="H22" s="6">
+        <v>0.578320004770153</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="B2:H2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated test for knot and db eval in overview doc
</commit_message>
<xml_diff>
--- a/doc/Document Tables.xlsx
+++ b/doc/Document Tables.xlsx
@@ -9,16 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="38475" yWindow="-1485" windowWidth="24480" windowHeight="17265" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="38475" yWindow="-1485" windowWidth="24480" windowHeight="17265" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Species" sheetId="1" r:id="rId1"/>
     <sheet name="CVs" sheetId="2" r:id="rId2"/>
+    <sheet name="Rho_Intercept Table" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Species!$A$1:$C$1</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="40">
   <si>
     <t>Region</t>
   </si>
@@ -109,6 +110,45 @@
   </si>
   <si>
     <t>VAST Model Knot Specification (n_x)</t>
+  </si>
+  <si>
+    <t>Rho_Intercept Name</t>
+  </si>
+  <si>
+    <t>FE</t>
+  </si>
+  <si>
+    <t>RW-FE</t>
+  </si>
+  <si>
+    <t>FE-RW</t>
+  </si>
+  <si>
+    <t>RW</t>
+  </si>
+  <si>
+    <t>AR-FE</t>
+  </si>
+  <si>
+    <t>FE-AR</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>Encounter Probability</t>
+  </si>
+  <si>
+    <t>Positive Catch Rate</t>
+  </si>
+  <si>
+    <t>Fixed effect</t>
+  </si>
+  <si>
+    <t>Random walk</t>
+  </si>
+  <si>
+    <t>Autoregressive (lag-1)</t>
   </si>
 </sst>
 </file>
@@ -195,21 +235,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="12" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="12" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -804,8 +841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:H22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -825,39 +862,39 @@
       <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="5">
+      <c r="B4" s="3">
         <v>100</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="3">
         <v>200</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="3">
         <v>300</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="3">
         <v>400</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="3">
         <v>500</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="3">
         <v>750</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="3">
         <v>1000</v>
       </c>
     </row>
@@ -865,25 +902,25 @@
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>-0.172033666650799</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>-0.21167461660944001</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>-0.20215163545793099</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>-0.20646862752263401</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <v>-0.21744322095305699</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <v>-0.225574064860074</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="5">
         <v>-0.23320697566235099</v>
       </c>
     </row>
@@ -891,25 +928,25 @@
       <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>-0.11659698793617999</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>-4.6655320264011903E-2</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>-8.2071749580468895E-2</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>-7.0225716441070701E-2</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <v>-4.9467660840880397E-2</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="5">
         <v>-5.8881687623085703E-2</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="5">
         <v>-7.9344830269770197E-2</v>
       </c>
     </row>
@@ -917,25 +954,25 @@
       <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>-0.47735462967118802</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>-0.47823423372074902</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>-0.48075111949067401</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>-0.47969377920014999</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <v>-0.48327084038687801</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="5">
         <v>-0.48347441893728699</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="5">
         <v>-0.484178785114243</v>
       </c>
     </row>
@@ -943,25 +980,25 @@
       <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>-0.42336225116582099</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>-0.42978829226184401</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>-0.43054175017481</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>-0.43857799323670599</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="5">
         <v>-0.4325395597992</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="5">
         <v>-0.41979056694823302</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="5">
         <v>-0.43260419909207998</v>
       </c>
     </row>
@@ -969,25 +1006,25 @@
       <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>-4.63700074382081E-2</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>-6.8470506145828003E-2</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>-8.7998193871509006E-2</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>-0.106271905976751</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="5">
         <v>-9.2243110105519804E-2</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="5">
         <v>-0.11261745542922399</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="5">
         <v>-0.11081741659528301</v>
       </c>
     </row>
@@ -995,25 +1032,25 @@
       <c r="A10" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <v>-7.5076824332551306E-2</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>-8.1504796751249803E-2</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <v>-9.2203344242930099E-2</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>-9.3549026531111995E-2</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="5">
         <v>-9.1131987033842399E-2</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="5">
         <v>-9.63153176291906E-2</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="5">
         <v>-0.100478582932572</v>
       </c>
     </row>
@@ -1021,25 +1058,25 @@
       <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <v>-0.30128172079058801</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>-0.30349258612034902</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="5">
         <v>-0.30685264037614002</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <v>-0.31988988759741599</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="5">
         <v>-0.31431787058965199</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="5">
         <v>-0.32794109500630803</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="5">
         <v>-0.31664385632049902</v>
       </c>
     </row>
@@ -1047,25 +1084,25 @@
       <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="5">
         <v>-8.1356792970777206E-2</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <v>-9.7225086063537497E-2</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="5">
         <v>-0.10581610184028099</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="5">
         <v>-0.110560470416739</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="5">
         <v>-0.12714521863946401</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="5">
         <v>-0.13859479025957</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="5">
         <v>-0.14532068629028799</v>
       </c>
     </row>
@@ -1073,25 +1110,25 @@
       <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <v>-0.45614395311852701</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <v>-0.46445351724316702</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="5">
         <v>-0.46712276524546797</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="5">
         <v>-0.47122980070753501</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="5">
         <v>-0.474878173128717</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="5">
         <v>-0.47602537920932803</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="5">
         <v>-0.47504208961909999</v>
       </c>
     </row>
@@ -1107,39 +1144,39 @@
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="3" t="s">
+      <c r="A16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="5">
+      <c r="B17" s="3">
         <v>100</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="3">
         <v>200</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="3">
         <v>300</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="3">
         <v>400</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="3">
         <v>500</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G17" s="3">
         <v>750</v>
       </c>
-      <c r="H17" s="5">
+      <c r="H17" s="3">
         <v>1000</v>
       </c>
     </row>
@@ -1147,25 +1184,25 @@
       <c r="A18" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="5">
         <v>0.40206667874438501</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="5">
         <v>0.35372882267482703</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="5">
         <v>0.279645426709414</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="5">
         <v>0.24555450887570501</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="5">
         <v>0.181530435316685</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G18" s="5">
         <v>0.21593836237153999</v>
       </c>
-      <c r="H18" s="6">
+      <c r="H18" s="5">
         <v>0.21721569551438</v>
       </c>
     </row>
@@ -1173,25 +1210,25 @@
       <c r="A19" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="5">
         <v>-8.8910240495234001E-3</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="5">
         <v>6.6898104923970997E-2</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="5">
         <v>-8.7022934231200805E-2</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="5">
         <v>-3.8570188579889399E-2</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="5">
         <v>-5.82454321445025E-2</v>
       </c>
-      <c r="G19" s="6">
+      <c r="G19" s="5">
         <v>-8.5155917447454793E-2</v>
       </c>
-      <c r="H19" s="6">
+      <c r="H19" s="5">
         <v>-0.10999567398181399</v>
       </c>
     </row>
@@ -1199,25 +1236,25 @@
       <c r="A20" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="5">
         <v>-0.249847546068524</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="5">
         <v>-0.22393092816979901</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="5">
         <v>-0.20901627755773999</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="5">
         <v>-0.23995942732798201</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="5">
         <v>-0.216851520715201</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G20" s="5">
         <v>-0.18802173950006901</v>
       </c>
-      <c r="H20" s="6">
+      <c r="H20" s="5">
         <v>-0.13592893757511301</v>
       </c>
     </row>
@@ -1225,25 +1262,25 @@
       <c r="A21" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="5">
         <v>-7.6866319208249698E-2</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="5">
         <v>-0.10581985445785</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="5">
         <v>-9.0342215364723005E-2</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="5">
         <v>-7.5435209305558804E-2</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F21" s="5">
         <v>-3.9874213705633502E-2</v>
       </c>
-      <c r="G21" s="6">
+      <c r="G21" s="5">
         <v>-7.4631440661902596E-2</v>
       </c>
-      <c r="H21" s="6">
+      <c r="H21" s="5">
         <v>-1.3432919863705199E-2</v>
       </c>
     </row>
@@ -1251,25 +1288,25 @@
       <c r="A22" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="5">
         <v>0.288065075752998</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="5">
         <v>0.49599574455914802</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="5">
         <v>0.47802532940015202</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="5">
         <v>0.49216163355298398</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="5">
         <v>0.49459423842366501</v>
       </c>
-      <c r="G22" s="6">
+      <c r="G22" s="5">
         <v>0.52037926494853104</v>
       </c>
-      <c r="H22" s="6">
+      <c r="H22" s="5">
         <v>0.578320004770153</v>
       </c>
     </row>
@@ -1283,4 +1320,112 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated figures for .doc
</commit_message>
<xml_diff>
--- a/doc/Document Tables.xlsx
+++ b/doc/Document Tables.xlsx
@@ -1,25 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\nmfs.local\AKC-ABL\Users\curry.cunningham\My Documents\Projects\VAST Evaluation\AFSC_VAST_Evaluation\doc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="38475" yWindow="-1485" windowWidth="24480" windowHeight="17265" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14640" windowHeight="20980" tabRatio="500" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Species" sheetId="1" r:id="rId1"/>
     <sheet name="CVs" sheetId="2" r:id="rId2"/>
     <sheet name="Rho_Intercept Table" sheetId="3" r:id="rId3"/>
+    <sheet name="Apportionment Table" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Species!$A$1:$C$1</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -29,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="48">
   <si>
     <t>Region</t>
   </si>
@@ -112,9 +108,6 @@
     <t>VAST Model Knot Specification (n_x)</t>
   </si>
   <si>
-    <t>Rho_Intercept Name</t>
-  </si>
-  <si>
     <t>FE</t>
   </si>
   <si>
@@ -149,6 +142,33 @@
   </si>
   <si>
     <t>Autoregressive (lag-1)</t>
+  </si>
+  <si>
+    <t>Rho_Intercept Notation</t>
+  </si>
+  <si>
+    <t>Notation</t>
+  </si>
+  <si>
+    <t>RW + IaY</t>
+  </si>
+  <si>
+    <t>AR + IaY</t>
+  </si>
+  <si>
+    <t>RW + AR</t>
+  </si>
+  <si>
+    <t>AR + RW</t>
+  </si>
+  <si>
+    <t>Spatio-temporal Random Effects</t>
+  </si>
+  <si>
+    <t>Independent among years</t>
+  </si>
+  <si>
+    <t>Intercepts</t>
   </si>
 </sst>
 </file>
@@ -220,7 +240,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -234,6 +254,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -242,14 +278,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="12" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="12" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -259,8 +295,24 @@
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="12" builtinId="5"/>
   </cellStyles>
@@ -651,14 +703,14 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.125" customWidth="1"/>
-    <col min="2" max="2" width="29.625" customWidth="1"/>
-    <col min="3" max="3" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -669,7 +721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -680,7 +732,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -691,7 +743,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -702,7 +754,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -713,7 +765,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -724,7 +776,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -735,7 +787,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -746,7 +798,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -757,7 +809,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -768,7 +820,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -779,7 +831,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -790,7 +842,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -801,7 +853,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -812,7 +864,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -845,37 +897,37 @@
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="17.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="1:8">
+      <c r="B2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8">
       <c r="B4" s="3">
         <v>100</v>
       </c>
@@ -898,266 +950,266 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>-0.172033666650799</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>-0.21167461660944001</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>-0.20215163545793099</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>-0.20646862752263401</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>-0.21744322095305699</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <v>-0.225574064860074</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="4">
         <v>-0.23320697566235099</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>-0.11659698793617999</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>-4.6655320264011903E-2</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>-8.2071749580468895E-2</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>-7.0225716441070701E-2</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>-4.9467660840880397E-2</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <v>-5.8881687623085703E-2</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="4">
         <v>-7.9344830269770197E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>-0.47735462967118802</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>-0.47823423372074902</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>-0.48075111949067401</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>-0.47969377920014999</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>-0.48327084038687801</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="4">
         <v>-0.48347441893728699</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="4">
         <v>-0.484178785114243</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>-0.42336225116582099</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>-0.42978829226184401</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>-0.43054175017481</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>-0.43857799323670599</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>-0.4325395597992</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="4">
         <v>-0.41979056694823302</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="4">
         <v>-0.43260419909207998</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <v>-4.63700074382081E-2</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>-6.8470506145828003E-2</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>-8.7998193871509006E-2</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <v>-0.106271905976751</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>-9.2243110105519804E-2</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="4">
         <v>-0.11261745542922399</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="4">
         <v>-0.11081741659528301</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <v>-7.5076824332551306E-2</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>-8.1504796751249803E-2</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>-9.2203344242930099E-2</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>-9.3549026531111995E-2</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <v>-9.1131987033842399E-2</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="4">
         <v>-9.63153176291906E-2</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="4">
         <v>-0.100478582932572</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="4">
         <v>-0.30128172079058801</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
         <v>-0.30349258612034902</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>-0.30685264037614002</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <v>-0.31988988759741599</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <v>-0.31431787058965199</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="4">
         <v>-0.32794109500630803</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="4">
         <v>-0.31664385632049902</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="4">
         <v>-8.1356792970777206E-2</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <v>-9.7225086063537497E-2</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>-0.10581610184028099</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="4">
         <v>-0.110560470416739</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="4">
         <v>-0.12714521863946401</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="4">
         <v>-0.13859479025957</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12" s="4">
         <v>-0.14532068629028799</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="4">
         <v>-0.45614395311852701</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <v>-0.46445351724316702</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <v>-0.46712276524546797</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="4">
         <v>-0.47122980070753501</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="4">
         <v>-0.474878173128717</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="4">
         <v>-0.47602537920932803</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H13" s="4">
         <v>-0.47504208961909999</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="4" t="s">
+    <row r="15" spans="1:8">
+      <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:8">
       <c r="B17" s="3">
         <v>100</v>
       </c>
@@ -1180,133 +1232,133 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="4">
         <v>0.40206667874438501</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="4">
         <v>0.35372882267482703</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="4">
         <v>0.279645426709414</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="4">
         <v>0.24555450887570501</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="4">
         <v>0.181530435316685</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G18" s="4">
         <v>0.21593836237153999</v>
       </c>
-      <c r="H18" s="5">
+      <c r="H18" s="4">
         <v>0.21721569551438</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="4">
         <v>-8.8910240495234001E-3</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="4">
         <v>6.6898104923970997E-2</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="4">
         <v>-8.7022934231200805E-2</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="4">
         <v>-3.8570188579889399E-2</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F19" s="4">
         <v>-5.82454321445025E-2</v>
       </c>
-      <c r="G19" s="5">
+      <c r="G19" s="4">
         <v>-8.5155917447454793E-2</v>
       </c>
-      <c r="H19" s="5">
+      <c r="H19" s="4">
         <v>-0.10999567398181399</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="4">
         <v>-0.249847546068524</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="4">
         <v>-0.22393092816979901</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="4">
         <v>-0.20901627755773999</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="4">
         <v>-0.23995942732798201</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F20" s="4">
         <v>-0.216851520715201</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G20" s="4">
         <v>-0.18802173950006901</v>
       </c>
-      <c r="H20" s="5">
+      <c r="H20" s="4">
         <v>-0.13592893757511301</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="4">
         <v>-7.6866319208249698E-2</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="4">
         <v>-0.10581985445785</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="4">
         <v>-9.0342215364723005E-2</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="4">
         <v>-7.5435209305558804E-2</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F21" s="4">
         <v>-3.9874213705633502E-2</v>
       </c>
-      <c r="G21" s="5">
+      <c r="G21" s="4">
         <v>-7.4631440661902596E-2</v>
       </c>
-      <c r="H21" s="5">
+      <c r="H21" s="4">
         <v>-1.3432919863705199E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="4">
         <v>0.288065075752998</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="4">
         <v>0.49599574455914802</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="4">
         <v>0.47802532940015202</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="4">
         <v>0.49216163355298398</v>
       </c>
-      <c r="F22" s="5">
+      <c r="F22" s="4">
         <v>0.49459423842366501</v>
       </c>
-      <c r="G22" s="5">
+      <c r="G22" s="4">
         <v>0.52037926494853104</v>
       </c>
-      <c r="H22" s="5">
+      <c r="H22" s="4">
         <v>0.578320004770153</v>
       </c>
     </row>
@@ -1318,7 +1370,12 @@
     <mergeCell ref="B2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1326,53 +1383,166 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
         <v>27</v>
       </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
         <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
         <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
         <v>37</v>
@@ -1381,51 +1551,24 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
         <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" t="s">
-        <v>39</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update description documents for 2017 data
</commit_message>
<xml_diff>
--- a/doc/Document Tables.xlsx
+++ b/doc/Document Tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14640" windowHeight="20980" tabRatio="500" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="1860" yWindow="7760" windowWidth="33600" windowHeight="20360" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Species" sheetId="1" r:id="rId1"/>
@@ -240,7 +240,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -270,8 +270,30 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -284,8 +306,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="51">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -303,6 +328,17 @@
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
@@ -313,6 +349,17 @@
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="12" builtinId="5"/>
   </cellStyles>
@@ -893,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="300" zoomScaleNormal="300" zoomScalePageLayoutView="300" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -903,50 +950,50 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="B4" s="3">
+      <c r="B4" s="5">
         <v>100</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="5">
         <v>200</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="5">
         <v>300</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="5">
         <v>400</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="5">
         <v>500</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="5">
         <v>750</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="5">
         <v>1000</v>
       </c>
     </row>
@@ -955,25 +1002,25 @@
         <v>1</v>
       </c>
       <c r="B5" s="4">
-        <v>-0.172033666650799</v>
+        <v>-0.17861900254506</v>
       </c>
       <c r="C5" s="4">
-        <v>-0.21167461660944001</v>
+        <v>-0.20411350816056201</v>
       </c>
       <c r="D5" s="4">
-        <v>-0.20215163545793099</v>
+        <v>-0.208305599925699</v>
       </c>
       <c r="E5" s="4">
-        <v>-0.20646862752263401</v>
+        <v>-0.204619269117189</v>
       </c>
       <c r="F5" s="4">
-        <v>-0.21744322095305699</v>
+        <v>-0.207682656943045</v>
       </c>
       <c r="G5" s="4">
-        <v>-0.225574064860074</v>
+        <v>-0.220448777068283</v>
       </c>
       <c r="H5" s="4">
-        <v>-0.23320697566235099</v>
+        <v>-0.22745913701442</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -981,25 +1028,25 @@
         <v>2</v>
       </c>
       <c r="B6" s="4">
-        <v>-0.11659698793617999</v>
+        <v>-0.15455631750697099</v>
       </c>
       <c r="C6" s="4">
-        <v>-4.6655320264011903E-2</v>
+        <v>-9.1932086100145E-2</v>
       </c>
       <c r="D6" s="4">
-        <v>-8.2071749580468895E-2</v>
+        <v>-8.6702439769863193E-2</v>
       </c>
       <c r="E6" s="4">
-        <v>-7.0225716441070701E-2</v>
+        <v>-8.3052270575961804E-2</v>
       </c>
       <c r="F6" s="4">
-        <v>-4.9467660840880397E-2</v>
+        <v>-0.12775363137540599</v>
       </c>
       <c r="G6" s="4">
-        <v>-5.8881687623085703E-2</v>
+        <v>-0.110939069840749</v>
       </c>
       <c r="H6" s="4">
-        <v>-7.9344830269770197E-2</v>
+        <v>-0.121023718284639</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1007,25 +1054,25 @@
         <v>3</v>
       </c>
       <c r="B7" s="4">
-        <v>-0.47735462967118802</v>
+        <v>-0.460568696375312</v>
       </c>
       <c r="C7" s="4">
-        <v>-0.47823423372074902</v>
+        <v>-0.46173855420476201</v>
       </c>
       <c r="D7" s="4">
-        <v>-0.48075111949067401</v>
+        <v>-0.46215434809878903</v>
       </c>
       <c r="E7" s="4">
-        <v>-0.47969377920014999</v>
+        <v>-0.464888467697467</v>
       </c>
       <c r="F7" s="4">
-        <v>-0.48327084038687801</v>
+        <v>-0.46553287648025998</v>
       </c>
       <c r="G7" s="4">
-        <v>-0.48347441893728699</v>
+        <v>-0.46552034337092502</v>
       </c>
       <c r="H7" s="4">
-        <v>-0.484178785114243</v>
+        <v>-0.46823243790309599</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1033,25 +1080,25 @@
         <v>4</v>
       </c>
       <c r="B8" s="4">
-        <v>-0.42336225116582099</v>
+        <v>-0.43082228532455402</v>
       </c>
       <c r="C8" s="4">
-        <v>-0.42978829226184401</v>
+        <v>-0.43376036099968102</v>
       </c>
       <c r="D8" s="4">
-        <v>-0.43054175017481</v>
+        <v>-0.43585698319110899</v>
       </c>
       <c r="E8" s="4">
-        <v>-0.43857799323670599</v>
+        <v>-0.44055330725105502</v>
       </c>
       <c r="F8" s="4">
-        <v>-0.4325395597992</v>
+        <v>-0.446430924301634</v>
       </c>
       <c r="G8" s="4">
-        <v>-0.41979056694823302</v>
+        <v>-0.43811014199370901</v>
       </c>
       <c r="H8" s="4">
-        <v>-0.43260419909207998</v>
+        <v>-0.42623912025562499</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1059,25 +1106,25 @@
         <v>5</v>
       </c>
       <c r="B9" s="4">
-        <v>-4.63700074382081E-2</v>
+        <v>-7.6650115341337297E-2</v>
       </c>
       <c r="C9" s="4">
-        <v>-6.8470506145828003E-2</v>
+        <v>-8.5982582706416094E-2</v>
       </c>
       <c r="D9" s="4">
-        <v>-8.7998193871509006E-2</v>
+        <v>-0.105648847881451</v>
       </c>
       <c r="E9" s="4">
-        <v>-0.106271905976751</v>
+        <v>-0.11967862686585599</v>
       </c>
       <c r="F9" s="4">
-        <v>-9.2243110105519804E-2</v>
+        <v>-0.12253069737345799</v>
       </c>
       <c r="G9" s="4">
-        <v>-0.11261745542922399</v>
+        <v>-0.119844045797051</v>
       </c>
       <c r="H9" s="4">
-        <v>-0.11081741659528301</v>
+        <v>-0.152476213535919</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1085,25 +1132,25 @@
         <v>6</v>
       </c>
       <c r="B10" s="4">
-        <v>-7.5076824332551306E-2</v>
+        <v>-6.6627593483111897E-2</v>
       </c>
       <c r="C10" s="4">
-        <v>-8.1504796751249803E-2</v>
+        <v>-8.0323983782851396E-2</v>
       </c>
       <c r="D10" s="4">
-        <v>-9.2203344242930099E-2</v>
+        <v>-8.4723127318613006E-2</v>
       </c>
       <c r="E10" s="4">
-        <v>-9.3549026531111995E-2</v>
+        <v>-8.6013799429883894E-2</v>
       </c>
       <c r="F10" s="4">
-        <v>-9.1131987033842399E-2</v>
+        <v>-8.6510632104899496E-2</v>
       </c>
       <c r="G10" s="4">
-        <v>-9.63153176291906E-2</v>
+        <v>-8.8889564137599797E-2</v>
       </c>
       <c r="H10" s="4">
-        <v>-0.100478582932572</v>
+        <v>-8.5632946386962797E-2</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1111,25 +1158,25 @@
         <v>8</v>
       </c>
       <c r="B11" s="4">
-        <v>-0.30128172079058801</v>
+        <v>-0.31594796908713502</v>
       </c>
       <c r="C11" s="4">
-        <v>-0.30349258612034902</v>
+        <v>-0.30898092961166701</v>
       </c>
       <c r="D11" s="4">
-        <v>-0.30685264037614002</v>
+        <v>-0.31728431955056002</v>
       </c>
       <c r="E11" s="4">
-        <v>-0.31988988759741599</v>
+        <v>-0.32710840143508302</v>
       </c>
       <c r="F11" s="4">
-        <v>-0.31431787058965199</v>
+        <v>-0.320514529076876</v>
       </c>
       <c r="G11" s="4">
-        <v>-0.32794109500630803</v>
+        <v>-0.32564740944097798</v>
       </c>
       <c r="H11" s="4">
-        <v>-0.31664385632049902</v>
+        <v>-0.33107798449232301</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1137,25 +1184,25 @@
         <v>9</v>
       </c>
       <c r="B12" s="4">
-        <v>-8.1356792970777206E-2</v>
+        <v>-5.9367763662280401E-2</v>
       </c>
       <c r="C12" s="4">
-        <v>-9.7225086063537497E-2</v>
+        <v>-7.5642692433395803E-2</v>
       </c>
       <c r="D12" s="4">
-        <v>-0.10581610184028099</v>
+        <v>-9.2085602097212699E-2</v>
       </c>
       <c r="E12" s="4">
-        <v>-0.110560470416739</v>
+        <v>-0.103649628767548</v>
       </c>
       <c r="F12" s="4">
-        <v>-0.12714521863946401</v>
+        <v>-0.113257331397626</v>
       </c>
       <c r="G12" s="4">
-        <v>-0.13859479025957</v>
+        <v>-0.125004392708993</v>
       </c>
       <c r="H12" s="4">
-        <v>-0.14532068629028799</v>
+        <v>-0.13945370376676999</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1163,51 +1210,51 @@
         <v>10</v>
       </c>
       <c r="B13" s="4">
-        <v>-0.45614395311852701</v>
+        <v>-0.455553370046688</v>
       </c>
       <c r="C13" s="4">
-        <v>-0.46445351724316702</v>
+        <v>-0.45769334814481399</v>
       </c>
       <c r="D13" s="4">
-        <v>-0.46712276524546797</v>
+        <v>-0.452182188459606</v>
       </c>
       <c r="E13" s="4">
-        <v>-0.47122980070753501</v>
+        <v>-0.45384958365633499</v>
       </c>
       <c r="F13" s="4">
-        <v>-0.474878173128717</v>
+        <v>-0.45776544832801602</v>
       </c>
       <c r="G13" s="4">
-        <v>-0.47602537920932803</v>
+        <v>-0.46260993890109797</v>
       </c>
       <c r="H13" s="4">
-        <v>-0.47504208961909999</v>
+        <v>-0.46807388913359399</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
     </row>
     <row r="17" spans="1:8">
       <c r="B17" s="3">
@@ -1237,25 +1284,25 @@
         <v>1</v>
       </c>
       <c r="B18" s="4">
-        <v>0.40206667874438501</v>
+        <v>0.40206531688847602</v>
       </c>
       <c r="C18" s="4">
-        <v>0.35372882267482703</v>
+        <v>0.35372640833999203</v>
       </c>
       <c r="D18" s="4">
-        <v>0.279645426709414</v>
+        <v>0.27964582352589101</v>
       </c>
       <c r="E18" s="4">
-        <v>0.24555450887570501</v>
+        <v>0.24555681975444801</v>
       </c>
       <c r="F18" s="4">
-        <v>0.181530435316685</v>
+        <v>0.18152955367733101</v>
       </c>
       <c r="G18" s="4">
-        <v>0.21593836237153999</v>
+        <v>0.21594187925004499</v>
       </c>
       <c r="H18" s="4">
-        <v>0.21721569551438</v>
+        <v>0.217218377300713</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -1263,25 +1310,25 @@
         <v>2</v>
       </c>
       <c r="B19" s="4">
-        <v>-8.8910240495234001E-3</v>
+        <v>-8.8937560634977895E-3</v>
       </c>
       <c r="C19" s="4">
-        <v>6.6898104923970997E-2</v>
+        <v>6.6897875358780695E-2</v>
       </c>
       <c r="D19" s="4">
-        <v>-8.7022934231200805E-2</v>
+        <v>-8.7022950022307796E-2</v>
       </c>
       <c r="E19" s="4">
-        <v>-3.8570188579889399E-2</v>
+        <v>-3.8571119264003799E-2</v>
       </c>
       <c r="F19" s="4">
-        <v>-5.82454321445025E-2</v>
+        <v>-5.8246439212139602E-2</v>
       </c>
       <c r="G19" s="4">
-        <v>-8.5155917447454793E-2</v>
+        <v>-8.5155366066490101E-2</v>
       </c>
       <c r="H19" s="4">
-        <v>-0.10999567398181399</v>
+        <v>-0.109994541017525</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1289,25 +1336,25 @@
         <v>3</v>
       </c>
       <c r="B20" s="4">
-        <v>-0.249847546068524</v>
+        <v>-0.249848596888575</v>
       </c>
       <c r="C20" s="4">
-        <v>-0.22393092816979901</v>
+        <v>-0.22393285411176</v>
       </c>
       <c r="D20" s="4">
-        <v>-0.20901627755773999</v>
+        <v>-0.20901500830459099</v>
       </c>
       <c r="E20" s="4">
-        <v>-0.23995942732798201</v>
+        <v>-0.23996182183966999</v>
       </c>
       <c r="F20" s="4">
-        <v>-0.216851520715201</v>
+        <v>-0.21685117261554299</v>
       </c>
       <c r="G20" s="4">
-        <v>-0.18802173950006901</v>
+        <v>-0.18802279989989901</v>
       </c>
       <c r="H20" s="4">
-        <v>-0.13592893757511301</v>
+        <v>-0.13592755087938199</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1315,25 +1362,25 @@
         <v>4</v>
       </c>
       <c r="B21" s="4">
-        <v>-7.6866319208249698E-2</v>
+        <v>-7.6864696050077896E-2</v>
       </c>
       <c r="C21" s="4">
-        <v>-0.10581985445785</v>
+        <v>-0.105820042178211</v>
       </c>
       <c r="D21" s="4">
-        <v>-9.0342215364723005E-2</v>
+        <v>-9.0338234463826494E-2</v>
       </c>
       <c r="E21" s="4">
-        <v>-7.5435209305558804E-2</v>
+        <v>-7.5431914268755396E-2</v>
       </c>
       <c r="F21" s="4">
-        <v>-3.9874213705633502E-2</v>
+        <v>-3.9877299895370401E-2</v>
       </c>
       <c r="G21" s="4">
-        <v>-7.4631440661902596E-2</v>
+        <v>-7.4632567661288299E-2</v>
       </c>
       <c r="H21" s="4">
-        <v>-1.3432919863705199E-2</v>
+        <v>-1.34320082898282E-2</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1341,25 +1388,25 @@
         <v>7</v>
       </c>
       <c r="B22" s="4">
-        <v>0.288065075752998</v>
+        <v>0.28806299185483802</v>
       </c>
       <c r="C22" s="4">
-        <v>0.49599574455914802</v>
+        <v>0.49599006036557702</v>
       </c>
       <c r="D22" s="4">
-        <v>0.47802532940015202</v>
+        <v>0.47802565028534</v>
       </c>
       <c r="E22" s="4">
-        <v>0.49216163355298398</v>
+        <v>0.49216064857016001</v>
       </c>
       <c r="F22" s="4">
-        <v>0.49459423842366501</v>
+        <v>0.49459405965940001</v>
       </c>
       <c r="G22" s="4">
-        <v>0.52037926494853104</v>
+        <v>0.52038057645482305</v>
       </c>
       <c r="H22" s="4">
-        <v>0.578320004770153</v>
+        <v>0.57832268197353698</v>
       </c>
     </row>
   </sheetData>
@@ -1497,7 +1544,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C5"/>
     </sheetView>
   </sheetViews>

</xml_diff>